<commit_message>
Homework 4 assignment updates
</commit_message>
<xml_diff>
--- a/NHANES_data_dictionary_homework.xlsx
+++ b/NHANES_data_dictionary_homework.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\Research\EPID 674\EPID674_Week2_Class\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Teaching/EPID674/2021_fall_online/Homework/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF41C206-2A94-4D2A-AE06-50F695EF3555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D2202ED3-5FB6-214A-B03E-8918CE3FB00B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C5EF0901-5797-40BB-A849-28BF0A615FC1}"/>
+    <workbookView xWindow="39940" yWindow="3520" windowWidth="19420" windowHeight="10420" xr2:uid="{C5EF0901-5797-40BB-A849-28BF0A615FC1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -144,9 +144,6 @@
     <t>NHANES Variable Created From</t>
   </si>
   <si>
-    <t>Five age groups</t>
-  </si>
-  <si>
     <t>Non-Hispanic White, Mexican American, Non-Hispanic Black, Other Hispanic, Other Race</t>
   </si>
   <si>
@@ -201,10 +198,13 @@
     <t>COT_H</t>
   </si>
   <si>
-    <t>[60,66.7], (66.7,73.3], (73.3,80]</t>
-  </si>
-  <si>
     <t>[60,66.7]</t>
+  </si>
+  <si>
+    <t>Four age groups</t>
+  </si>
+  <si>
+    <t>[60, 65], (65, 70], (70, 75],  (75, 80]</t>
   </si>
 </sst>
 </file>
@@ -576,18 +576,18 @@
       <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.54296875" customWidth="1"/>
-    <col min="2" max="2" width="27.81640625" customWidth="1"/>
-    <col min="3" max="3" width="13.1796875" customWidth="1"/>
-    <col min="4" max="4" width="32.26953125" customWidth="1"/>
-    <col min="5" max="5" width="19.1796875" customWidth="1"/>
-    <col min="6" max="6" width="8.54296875" customWidth="1"/>
-    <col min="7" max="7" width="27.54296875" customWidth="1"/>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="27.83203125" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
+    <col min="4" max="4" width="32.33203125" customWidth="1"/>
+    <col min="5" max="5" width="19.1640625" customWidth="1"/>
+    <col min="6" max="6" width="8.5" customWidth="1"/>
+    <col min="7" max="7" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -613,7 +613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -636,10 +636,10 @@
         <v>6</v>
       </c>
       <c r="H2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -662,10 +662,10 @@
         <v>17</v>
       </c>
       <c r="H3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -688,24 +688,24 @@
         <v>8</v>
       </c>
       <c r="H4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="C5" t="s">
         <v>32</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F5" t="s">
         <v>29</v>
@@ -714,10 +714,10 @@
         <v>8</v>
       </c>
       <c r="H5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -728,7 +728,7 @@
         <v>32</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s">
         <v>28</v>
@@ -740,10 +740,10 @@
         <v>16</v>
       </c>
       <c r="H6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -766,10 +766,10 @@
         <v>11</v>
       </c>
       <c r="H7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -780,7 +780,7 @@
         <v>32</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E8" t="s">
         <v>34</v>
@@ -792,10 +792,10 @@
         <v>15</v>
       </c>
       <c r="H8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -818,10 +818,10 @@
         <v>13</v>
       </c>
       <c r="H9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -844,15 +844,15 @@
         <v>14</v>
       </c>
       <c r="H10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="C11" t="s">
         <v>33</v>
@@ -867,18 +867,18 @@
         <v>7</v>
       </c>
       <c r="G11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
         <v>33</v>
@@ -890,21 +890,21 @@
         <v>7</v>
       </c>
       <c r="F12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" t="s">
+        <v>38</v>
+      </c>
+      <c r="H12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="G12" t="s">
-        <v>39</v>
-      </c>
-      <c r="H12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="C13" t="s">
         <v>33</v>
@@ -916,21 +916,21 @@
         <v>7</v>
       </c>
       <c r="F13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>40</v>
       </c>
-      <c r="H13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>41</v>
-      </c>
       <c r="B14" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
         <v>33</v>
@@ -942,13 +942,13 @@
         <v>7</v>
       </c>
       <c r="F14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>